<commit_message>
Auto log-in, refactors, added services
Automatically log in with the admin user, clean up of some test code, added service calls to the tciaService file.
</commit_message>
<xml_diff>
--- a/tcia-submission-template.xlsx
+++ b/tcia-submission-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliefrund/Documents/Projects/TCIA-Submission-UI-Angular/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliefrund/JavaPrograms/CTP/ROOT/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Local Patient ID</t>
   </si>
@@ -42,6 +42,18 @@
   </si>
   <si>
     <t>TCGA-BLCA</t>
+  </si>
+  <si>
+    <t>TCGA-12-5436</t>
+  </si>
+  <si>
+    <t>CPTAC-UCEC-0001</t>
+  </si>
+  <si>
+    <t>CPTAC-Uterine</t>
+  </si>
+  <si>
+    <t>CPTAC-UCEC-0002</t>
   </si>
   <si>
     <t>ptid</t>
@@ -372,7 +384,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -385,13 +397,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -405,7 +417,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -423,13 +435,46 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D4" s="1"/>
+      <c r="A4">
+        <v>7980790</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>39181</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D5" s="1"/>
+      <c r="A5">
+        <v>12348975</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1">
+        <v>42825</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D6" s="1"/>
+      <c r="A6">
+        <v>13497812</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1">
+        <v>42825</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>